<commit_message>
add scatter for best and worst casee in all experiments
</commit_message>
<xml_diff>
--- a/S4/CKDN_content.xlsx
+++ b/S4/CKDN_content.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OTHER\ترم 3\پایاننامه\proposal\knowledge distillation\CKDN_code\S4\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -244,8 +249,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,7 +287,172 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>20675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="381001"/>
+          <a:ext cx="3276600" cy="2878174"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>76869</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19505</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12868275" y="400050"/>
+          <a:ext cx="3058194" cy="2857955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>6727</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9163050" y="3609975"/>
+          <a:ext cx="3035677" cy="2886075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>38730</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>88468</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12839700" y="3600450"/>
+          <a:ext cx="3048630" cy="2965018"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -328,7 +498,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -360,9 +530,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -394,6 +565,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -569,14 +741,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E4:F298"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="5:6">
+    <row r="4" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>0</v>
       </c>
@@ -584,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="5:6">
+    <row r="5" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>3</v>
       </c>
@@ -592,7 +766,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="5:6">
+    <row r="6" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>6</v>
       </c>
@@ -600,7 +774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="5:6">
+    <row r="7" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>9</v>
       </c>
@@ -608,7 +782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="5:6">
+    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>12</v>
       </c>
@@ -616,7 +790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="5:6">
+    <row r="9" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>15</v>
       </c>
@@ -624,7 +798,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="5:6">
+    <row r="10" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>18</v>
       </c>
@@ -632,7 +806,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="5:6">
+    <row r="11" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>21</v>
       </c>
@@ -640,7 +814,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="5:6">
+    <row r="12" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>24</v>
       </c>
@@ -648,7 +822,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="5:6">
+    <row r="13" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>27</v>
       </c>
@@ -656,7 +830,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="5:6">
+    <row r="14" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>30</v>
       </c>
@@ -664,7 +838,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="5:6">
+    <row r="15" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>33</v>
       </c>
@@ -672,7 +846,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="5:6">
+    <row r="16" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>36</v>
       </c>
@@ -680,7 +854,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="5:6">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>39</v>
       </c>
@@ -688,7 +862,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="5:6">
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>42</v>
       </c>
@@ -696,7 +870,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="5:6">
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>45</v>
       </c>
@@ -704,7 +878,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="5:6">
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>48</v>
       </c>
@@ -712,7 +886,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="5:6">
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>51</v>
       </c>
@@ -720,7 +894,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="5:6">
+    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>54</v>
       </c>
@@ -728,7 +902,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="5:6">
+    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>57</v>
       </c>
@@ -736,7 +910,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="5:6">
+    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>60</v>
       </c>
@@ -744,7 +918,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="5:6">
+    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>63</v>
       </c>
@@ -752,7 +926,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="5:6">
+    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>66</v>
       </c>
@@ -760,7 +934,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="5:6">
+    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>69</v>
       </c>
@@ -768,7 +942,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="5:6">
+    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>72</v>
       </c>
@@ -776,7 +950,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="274" spans="5:6">
+    <row r="274" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E274" t="s">
         <v>0</v>
       </c>
@@ -784,7 +958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="275" spans="5:6">
+    <row r="275" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E275" t="s">
         <v>3</v>
       </c>
@@ -792,7 +966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="5:6">
+    <row r="276" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E276" t="s">
         <v>6</v>
       </c>
@@ -800,7 +974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="277" spans="5:6">
+    <row r="277" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E277" t="s">
         <v>9</v>
       </c>
@@ -808,7 +982,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="278" spans="5:6">
+    <row r="278" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E278" t="s">
         <v>12</v>
       </c>
@@ -816,7 +990,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="279" spans="5:6">
+    <row r="279" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E279" t="s">
         <v>15</v>
       </c>
@@ -824,7 +998,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="280" spans="5:6">
+    <row r="280" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E280" t="s">
         <v>18</v>
       </c>
@@ -832,7 +1006,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="281" spans="5:6">
+    <row r="281" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E281" t="s">
         <v>21</v>
       </c>
@@ -840,7 +1014,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="282" spans="5:6">
+    <row r="282" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E282" t="s">
         <v>24</v>
       </c>
@@ -848,7 +1022,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="283" spans="5:6">
+    <row r="283" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E283" t="s">
         <v>27</v>
       </c>
@@ -856,7 +1030,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="284" spans="5:6">
+    <row r="284" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E284" t="s">
         <v>30</v>
       </c>
@@ -864,7 +1038,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="285" spans="5:6">
+    <row r="285" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E285" t="s">
         <v>33</v>
       </c>
@@ -872,7 +1046,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="286" spans="5:6">
+    <row r="286" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E286" t="s">
         <v>36</v>
       </c>
@@ -880,7 +1054,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="287" spans="5:6">
+    <row r="287" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E287" t="s">
         <v>39</v>
       </c>
@@ -888,7 +1062,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="288" spans="5:6">
+    <row r="288" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E288" t="s">
         <v>42</v>
       </c>
@@ -896,7 +1070,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="289" spans="5:6">
+    <row r="289" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E289" t="s">
         <v>45</v>
       </c>
@@ -904,7 +1078,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="290" spans="5:6">
+    <row r="290" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E290" t="s">
         <v>48</v>
       </c>
@@ -912,7 +1086,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="291" spans="5:6">
+    <row r="291" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E291" t="s">
         <v>51</v>
       </c>
@@ -920,7 +1094,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="292" spans="5:6">
+    <row r="292" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E292" t="s">
         <v>54</v>
       </c>
@@ -928,7 +1102,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="293" spans="5:6">
+    <row r="293" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E293" t="s">
         <v>57</v>
       </c>
@@ -936,7 +1110,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="294" spans="5:6">
+    <row r="294" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E294" t="s">
         <v>60</v>
       </c>
@@ -944,7 +1118,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="295" spans="5:6">
+    <row r="295" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E295" t="s">
         <v>63</v>
       </c>
@@ -952,7 +1126,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="296" spans="5:6">
+    <row r="296" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E296" t="s">
         <v>66</v>
       </c>
@@ -960,7 +1134,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="297" spans="5:6">
+    <row r="297" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E297" t="s">
         <v>69</v>
       </c>
@@ -968,7 +1142,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="298" spans="5:6">
+    <row r="298" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E298" t="s">
         <v>72</v>
       </c>
@@ -978,5 +1152,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>